<commit_message>
updated mark to 51.5/52
</commit_message>
<xml_diff>
--- a/deliverables/asn2/asn2_marking_scheme - Copy.xlsx
+++ b/deliverables/asn2/asn2_marking_scheme - Copy.xlsx
@@ -1046,7 +1046,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1379,7 +1379,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="38">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="D29" s="16" t="s">
         <v>35</v>
@@ -1445,7 +1445,7 @@
       </c>
       <c r="C34" s="38">
         <f>SUM(C28:C33)</f>
-        <v>29</v>
+        <v>29.5</v>
       </c>
       <c r="D34" s="17"/>
     </row>
@@ -1462,7 +1462,7 @@
       </c>
       <c r="C36" s="32">
         <f>SUM(C6,C11,C16,C23,C26,C34)</f>
-        <v>51</v>
+        <v>51.5</v>
       </c>
       <c r="D36" s="30"/>
     </row>
@@ -1473,7 +1473,7 @@
       <c r="B37" s="29"/>
       <c r="C37" s="33">
         <f>C36/B36</f>
-        <v>0.98076923076923073</v>
+        <v>0.99038461538461542</v>
       </c>
       <c r="D37" s="30"/>
     </row>
@@ -1484,7 +1484,7 @@
       <c r="B38" s="29"/>
       <c r="C38" s="32">
         <f>C37*7</f>
-        <v>6.865384615384615</v>
+        <v>6.9326923076923084</v>
       </c>
       <c r="D38" s="30"/>
     </row>

</xml_diff>